<commit_message>
added to excel using specified location
</commit_message>
<xml_diff>
--- a/videos.xlsx
+++ b/videos.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E1"/>
+  <dimension ref="A2:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -421,28 +421,28 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
+    <row r="2">
+      <c r="A2" t="inlineStr">
         <is>
           <t>ID</t>
         </is>
       </c>
-      <c r="B1" t="inlineStr">
+      <c r="B2" t="inlineStr">
         <is>
           <t>URL</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
+      <c r="C2" t="inlineStr">
         <is>
           <t>Type</t>
         </is>
       </c>
-      <c r="D1" t="inlineStr">
+      <c r="D2" t="inlineStr">
         <is>
           <t>Created Date</t>
         </is>
       </c>
-      <c r="E1" t="inlineStr">
+      <c r="E2" t="inlineStr">
         <is>
           <t>Download Date</t>
         </is>

</xml_diff>

<commit_message>
Comments different for each heading
</commit_message>
<xml_diff>
--- a/videos.xlsx
+++ b/videos.xlsx
@@ -187,27 +187,27 @@
   <commentList>
     <comment ref="A1" authorId="0" shapeId="0">
       <text>
-        <t>This is a heading</t>
+        <t>This is the unique identifier for each row</t>
       </text>
     </comment>
     <comment ref="B1" authorId="0" shapeId="0">
       <text>
-        <t>This is a heading</t>
+        <t>This is the URL for the video</t>
       </text>
     </comment>
     <comment ref="C1" authorId="0" shapeId="0">
       <text>
-        <t>This is a heading</t>
+        <t>This is the download type for the video</t>
       </text>
     </comment>
     <comment ref="D1" authorId="0" shapeId="0">
       <text>
-        <t>This is a heading</t>
+        <t>This is the date that the entry was created</t>
       </text>
     </comment>
     <comment ref="E1" authorId="0" shapeId="0">
       <text>
-        <t>This is a heading</t>
+        <t>This is the date that the video was downloaded (if applicable)</t>
       </text>
     </comment>
   </commentList>

</xml_diff>

<commit_message>
Fit to data size
</commit_message>
<xml_diff>
--- a/videos.xlsx
+++ b/videos.xlsx
@@ -512,9 +512,9 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="4.8" customWidth="1" min="1" max="1"/>
-    <col width="6" customWidth="1" min="2" max="2"/>
-    <col width="7.199999999999999" customWidth="1" min="3" max="3"/>
-    <col width="16.8" customWidth="1" min="4" max="4"/>
+    <col width="45" customWidth="1" min="2" max="2"/>
+    <col width="10" customWidth="1" min="3" max="3"/>
+    <col width="19" customWidth="1" min="4" max="4"/>
     <col width="18" customWidth="1" min="5" max="5"/>
   </cols>
   <sheetData>

</xml_diff>